<commit_message>
arrays - p8 completed
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siddh\Desktop\PROJECT CP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siddh\Desktop\PROJECT CP\dsa-practice-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A10ABE5-4621-4C48-931B-9BD58929BA1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C8E45B-A754-4135-B003-FB3BB820FB81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1896,8 +1896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2037,8 +2037,8 @@
       <c r="B12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>4</v>
+      <c r="C12" s="12" t="s">
+        <v>465</v>
       </c>
       <c r="D12" s="2">
         <v>7</v>

</xml_diff>

<commit_message>
attempted p10 with linear time
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siddh\Desktop\PROJECT CP\dsa-practice-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C1B6E2-2480-4CB6-9F40-78A29B3AF67B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B05B34-0AB8-41F2-BF08-25B574FA3F46}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1428,10 +1428,10 @@
     <t>*</t>
   </si>
   <si>
-    <t>stuck</t>
-  </si>
-  <si>
     <t>need to rethink</t>
+  </si>
+  <si>
+    <t>attempting…</t>
   </si>
 </sst>
 </file>
@@ -1936,8 +1936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1945,6 +1945,7 @@
     <col min="1" max="1" width="24.8984375" customWidth="1"/>
     <col min="2" max="2" width="116.69921875" customWidth="1"/>
     <col min="3" max="3" width="19.8984375" customWidth="1"/>
+    <col min="4" max="4" width="5.296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="24.6">
@@ -2103,8 +2104,8 @@
       <c r="B14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>467</v>
+      <c r="C14" s="12" t="s">
+        <v>465</v>
       </c>
       <c r="D14" s="2">
         <v>9</v>
@@ -2118,7 +2119,7 @@
         <v>15</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D15" s="2">
         <v>10</v>
@@ -2131,8 +2132,8 @@
       <c r="B16" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="13" t="s">
-        <v>4</v>
+      <c r="C16" s="14" t="s">
+        <v>468</v>
       </c>
       <c r="D16" s="2">
         <v>11</v>
@@ -2145,8 +2146,8 @@
       <c r="B17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="13" t="s">
-        <v>4</v>
+      <c r="C17" s="14" t="s">
+        <v>468</v>
       </c>
       <c r="D17" s="2">
         <v>12</v>

</xml_diff>

<commit_message>
solved p15 and did some minor modifications in other codes
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siddh\Desktop\PROJECT CP\dsa-practice-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B05B34-0AB8-41F2-BF08-25B574FA3F46}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C437C8-D3BA-4612-A711-58A0417F35CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="471">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1428,10 +1428,17 @@
     <t>*</t>
   </si>
   <si>
-    <t>need to rethink</t>
-  </si>
-  <si>
-    <t>attempting…</t>
+    <t>need to understand correctness of linear solution</t>
+  </si>
+  <si>
+    <t>need to understand core problem: start of loop in linked list,
+reconsider the mathematical proof</t>
+  </si>
+  <si>
+    <t>need correctness intuition for reodering algorithm</t>
+  </si>
+  <si>
+    <t>need to optimize for space complexity</t>
   </si>
 </sst>
 </file>
@@ -1582,7 +1589,7 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1615,6 +1622,18 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1936,15 +1955,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="24.8984375" customWidth="1"/>
-    <col min="2" max="2" width="116.69921875" customWidth="1"/>
-    <col min="3" max="3" width="19.8984375" customWidth="1"/>
+    <col min="2" max="2" width="103.69921875" customWidth="1"/>
+    <col min="3" max="3" width="47.8984375" customWidth="1"/>
     <col min="4" max="4" width="5.296875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2125,17 +2144,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="21">
-      <c r="A16" s="7" t="s">
+    <row r="16" spans="1:4" ht="40.799999999999997" customHeight="1">
+      <c r="A16" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="18" t="s">
         <v>468</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="17">
         <v>11</v>
       </c>
     </row>
@@ -2147,7 +2166,7 @@
         <v>17</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D17" s="2">
         <v>12</v>
@@ -2160,8 +2179,8 @@
       <c r="B18" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="13" t="s">
-        <v>4</v>
+      <c r="C18" s="12" t="s">
+        <v>465</v>
       </c>
       <c r="D18" s="2">
         <v>13</v>
@@ -2174,8 +2193,8 @@
       <c r="B19" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="13" t="s">
-        <v>4</v>
+      <c r="C19" s="14" t="s">
+        <v>470</v>
       </c>
       <c r="D19" s="2">
         <v>14</v>

</xml_diff>

<commit_message>
solved p16 with merge algo
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siddh\Desktop\PROJECT CP\dsa-practice-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B25D40-BE9B-4D2E-9419-18FD03119B96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4121F5BA-9DA8-4272-A037-B82D085895DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1956,7 +1956,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2221,8 +2221,8 @@
       <c r="B21" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="13" t="s">
-        <v>4</v>
+      <c r="C21" s="12" t="s">
+        <v>465</v>
       </c>
       <c r="D21" s="2">
         <v>16</v>

</xml_diff>

<commit_message>
solved  p17 in linear time
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siddh\Desktop\PROJECT CP\dsa-practice-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4121F5BA-9DA8-4272-A037-B82D085895DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A6F41F0-983B-4A16-A609-0DD2F3FE593E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1955,7 +1955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
solved arrays:p19 in linear time
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siddh\Desktop\PROJECT CP\dsa-practice-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A6F41F0-983B-4A16-A609-0DD2F3FE593E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0539AC1-664D-4E72-9BB3-99EC1239C137}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1955,8 +1955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2235,8 +2235,8 @@
       <c r="B22" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="13" t="s">
-        <v>4</v>
+      <c r="C22" s="12" t="s">
+        <v>465</v>
       </c>
       <c r="D22" s="2">
         <v>17</v>
@@ -2249,8 +2249,8 @@
       <c r="B23" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="13" t="s">
-        <v>4</v>
+      <c r="C23" s="12" t="s">
+        <v>465</v>
       </c>
       <c r="D23" s="2">
         <v>18</v>
@@ -2263,8 +2263,8 @@
       <c r="B24" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="13" t="s">
-        <v>4</v>
+      <c r="C24" s="12" t="s">
+        <v>465</v>
       </c>
       <c r="D24" s="2">
         <v>19</v>

</xml_diff>

<commit_message>
solved arrays:p25 with hashmap in linear time
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siddh\Desktop\PROJECT CP\dsa-practice-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B677FD-ABA1-482A-ABF7-15D38D915DAB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347C3381-27BB-468D-BFFC-9DF313A164AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="473">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1442,6 +1442,9 @@
   </si>
   <si>
     <t>done in qudratic time</t>
+  </si>
+  <si>
+    <t>solved with hashmap</t>
   </si>
 </sst>
 </file>
@@ -1958,8 +1961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="B24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2351,8 +2354,8 @@
       <c r="B30" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="13" t="s">
-        <v>4</v>
+      <c r="C30" s="14" t="s">
+        <v>472</v>
       </c>
       <c r="D30" s="6">
         <v>25</v>

</xml_diff>

<commit_message>
solved arrays:p26 and p27
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siddh\Desktop\PROJECT CP\dsa-practice-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347C3381-27BB-468D-BFFC-9DF313A164AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0B5309-FA60-409D-8285-85B603BC719F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1961,8 +1961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2382,8 +2382,8 @@
       <c r="B32" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="13" t="s">
-        <v>4</v>
+      <c r="C32" s="12" t="s">
+        <v>465</v>
       </c>
       <c r="D32" s="6">
         <v>27</v>

</xml_diff>